<commit_message>
adding all scripts, results, models to abby branch
</commit_message>
<xml_diff>
--- a/data/Data Dictionary.xlsx
+++ b/data/Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cd28d252529c2a2/Documents/GitHub/wids_project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharadak/Documents/wids/2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{CE36A37A-529F-C24C-BF1C-E0B715FD200E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95926FC0-6D56-4262-9A84-C893767F7ADC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE36A37A-529F-C24C-BF1C-E0B715FD200E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A119C154-C5C6-4A39-B58B-073FBEBDAF9F}"/>
+    <workbookView xWindow="3600" yWindow="1600" windowWidth="35840" windowHeight="20800" xr2:uid="{A119C154-C5C6-4A39-B58B-073FBEBDAF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
@@ -81,6 +81,13 @@
     <t>categorical int</t>
   </si>
   <si>
+    <t>1=Staten Island 
+2=MRV
+3=Midtown
+4=Harlem
+5=SI RUMC</t>
+  </si>
+  <si>
     <t>float</t>
   </si>
   <si>
@@ -143,6 +150,12 @@
     <t>Scan location</t>
   </si>
   <si>
+    <t>1=Staten Island
+2=RUBIC
+3=CBIC
+4=CUNY</t>
+  </si>
+  <si>
     <t>Ishihara Color Vision Test</t>
   </si>
   <si>
@@ -699,19 +712,6 @@
   </si>
   <si>
     <t>0= Other/None, 1=ADHD</t>
-  </si>
-  <si>
-    <t>1=Staten Island 
-2=MRV (Manhattan Radiology and Vascular?)
-3=Midtown
-4=Harlem
-5=SI RUMC (Staten Island Richmond University Medical Center?)</t>
-  </si>
-  <si>
-    <t>1=Staten Island
-2=RUBIC (Rutgers University Brain Imaging Center?)
-3=CBIC (Center for Brain Imaging and Connectivity or Cognitive Brain Imaging Center?)
-4=CUNY (City University of New York?)</t>
   </si>
 </sst>
 </file>
@@ -777,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -792,7 +792,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,23 +1128,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FBF5DF4-B011-43DD-B358-28254206D7AD}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="116.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="116.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1164,9 +1163,9 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1175,12 +1174,12 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1189,327 +1188,327 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
         <v>189</v>
       </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" t="s">
-        <v>187</v>
-      </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1518,15 +1517,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
@@ -1535,15 +1534,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -1552,192 +1551,192 @@
         <v>12</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="192" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="195" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>193</v>
-      </c>
-      <c r="B31" t="s">
-        <v>37</v>
-      </c>
       <c r="C31" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="192" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>195</v>
+      </c>
+      <c r="B33" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="195" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B33" t="s">
-        <v>37</v>
-      </c>
       <c r="C33" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C37" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E37" t="s">
         <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C38" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1753,82 +1752,82 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.140625" customWidth="1"/>
-    <col min="2" max="2" width="78.42578125" customWidth="1"/>
+    <col min="1" max="1" width="54.1640625" customWidth="1"/>
+    <col min="2" max="2" width="78.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1838,152 +1837,147 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCDC3DE-66FC-48A6-942D-324BFB2788C5}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
         <v>70</v>
       </c>
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
         <v>81</v>
       </c>
-      <c r="B15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1994,363 +1988,363 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139884C0-9B28-4B5A-96AE-7647E2A6AADD}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="119.140625" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" customWidth="1"/>
+    <col min="1" max="1" width="119.1640625" customWidth="1"/>
+    <col min="2" max="2" width="58.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B37" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2366,287 +2360,287 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="144.140625" customWidth="1"/>
-    <col min="2" max="2" width="131.42578125" customWidth="1"/>
+    <col min="1" max="1" width="144.1640625" customWidth="1"/>
+    <col min="2" max="2" width="131.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" t="s">
         <v>134</v>
       </c>
-      <c r="B5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>